<commit_message>
this is so fucking good
</commit_message>
<xml_diff>
--- a/Copy.xlsx
+++ b/Copy.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="19200" yWindow="0" windowWidth="19200" windowHeight="21000" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Аркуш1" sheetId="1" state="visible" r:id="rId1"/>
@@ -394,7 +394,7 @@
   <dimension ref="A1:G1105"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+      <selection activeCell="AF13" sqref="AF13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -1030,6 +1030,21 @@
       <c r="A42" s="1" t="n">
         <v>45026</v>
       </c>
+      <c r="B42" t="n">
+        <v>56</v>
+      </c>
+      <c r="C42" t="n">
+        <v>584</v>
+      </c>
+      <c r="D42" t="n">
+        <v>131</v>
+      </c>
+      <c r="E42" t="n">
+        <v>3680</v>
+      </c>
+      <c r="F42" t="n">
+        <v>265</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="n">

</xml_diff>

<commit_message>
this is so good
</commit_message>
<xml_diff>
--- a/Copy.xlsx
+++ b/Copy.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Аркуш1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Аркуш1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
@@ -45,9 +45,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Звичайний" xfId="0" builtinId="0"/>
@@ -391,10 +394,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1105"/>
+  <dimension ref="A1:H1105"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AF13" sqref="AF13"/>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="U105" sqref="U105:U106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -553,13 +556,16 @@
         <v>44994</v>
       </c>
       <c r="B10" t="n">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C10" t="n">
         <v>402</v>
       </c>
       <c r="D10" t="n">
         <v>77</v>
+      </c>
+      <c r="E10" t="n">
+        <v>2403</v>
       </c>
     </row>
     <row r="11">
@@ -567,13 +573,21 @@
         <v>44995</v>
       </c>
       <c r="B11" t="n">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C11" t="n">
         <v>419</v>
       </c>
       <c r="D11" t="n">
         <v>80</v>
+      </c>
+      <c r="E11" t="n">
+        <v>2456</v>
+      </c>
+      <c r="H11" s="2" t="inlineStr">
+        <is>
+          <t>ФІКЦІЯ, ДОДАНО ШТУЧНО, НЕ Є РЕАЬНИМИ ДАНИМИ</t>
+        </is>
       </c>
     </row>
     <row r="12">
@@ -581,13 +595,16 @@
         <v>44996</v>
       </c>
       <c r="B12" t="n">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C12" t="n">
         <v>396</v>
       </c>
       <c r="D12" t="n">
         <v>70</v>
+      </c>
+      <c r="E12" t="n">
+        <v>2495</v>
       </c>
     </row>
     <row r="13">
@@ -595,13 +612,16 @@
         <v>44997</v>
       </c>
       <c r="B13" t="n">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C13" t="n">
         <v>247</v>
       </c>
       <c r="D13" t="n">
         <v>34</v>
+      </c>
+      <c r="E13" t="n">
+        <v>2507</v>
       </c>
     </row>
     <row r="14">
@@ -609,13 +629,16 @@
         <v>44998</v>
       </c>
       <c r="B14" t="n">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C14" t="n">
         <v>480</v>
       </c>
       <c r="D14" t="n">
         <v>86</v>
+      </c>
+      <c r="E14" t="n">
+        <v>2583</v>
       </c>
     </row>
     <row r="15">
@@ -623,13 +646,16 @@
         <v>44999</v>
       </c>
       <c r="B15" t="n">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C15" t="n">
         <v>425</v>
       </c>
       <c r="D15" t="n">
         <v>71</v>
+      </c>
+      <c r="E15" t="n">
+        <v>2625</v>
       </c>
     </row>
     <row r="16">
@@ -637,13 +663,16 @@
         <v>45000</v>
       </c>
       <c r="B16" t="n">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C16" t="n">
         <v>254</v>
       </c>
       <c r="D16" t="n">
         <v>39</v>
+      </c>
+      <c r="E16" t="n">
+        <v>2653</v>
       </c>
     </row>
     <row r="17">
@@ -651,13 +680,16 @@
         <v>45001</v>
       </c>
       <c r="B17" t="n">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C17" t="n">
         <v>379</v>
       </c>
       <c r="D17" t="n">
         <v>62</v>
+      </c>
+      <c r="E17" t="n">
+        <v>2702</v>
       </c>
     </row>
     <row r="18">
@@ -665,13 +697,16 @@
         <v>45002</v>
       </c>
       <c r="B18" t="n">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C18" t="n">
         <v>535</v>
       </c>
       <c r="D18" t="n">
         <v>97</v>
+      </c>
+      <c r="E18" t="n">
+        <v>2777</v>
       </c>
     </row>
     <row r="19">
@@ -679,13 +714,16 @@
         <v>45003</v>
       </c>
       <c r="B19" t="n">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C19" t="n">
         <v>381</v>
       </c>
       <c r="D19" t="n">
         <v>61</v>
+      </c>
+      <c r="E19" t="n">
+        <v>2815</v>
       </c>
     </row>
     <row r="20">
@@ -693,13 +731,16 @@
         <v>45004</v>
       </c>
       <c r="B20" t="n">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="C20" t="n">
         <v>334</v>
       </c>
       <c r="D20" t="n">
         <v>58</v>
+      </c>
+      <c r="E20" t="n">
+        <v>2843</v>
       </c>
     </row>
     <row r="21">
@@ -707,13 +748,16 @@
         <v>45005</v>
       </c>
       <c r="B21" t="n">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C21" t="n">
         <v>438</v>
       </c>
       <c r="D21" t="n">
         <v>73</v>
+      </c>
+      <c r="E21" t="n">
+        <v>2877</v>
       </c>
     </row>
     <row r="22">
@@ -721,13 +765,16 @@
         <v>45006</v>
       </c>
       <c r="B22" t="n">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C22" t="n">
         <v>367</v>
       </c>
       <c r="D22" t="n">
         <v>60</v>
+      </c>
+      <c r="E22" t="n">
+        <v>2954</v>
       </c>
     </row>
     <row r="23">
@@ -735,13 +782,16 @@
         <v>45007</v>
       </c>
       <c r="B23" t="n">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C23" t="n">
         <v>637</v>
       </c>
       <c r="D23" t="n">
         <v>113</v>
+      </c>
+      <c r="E23" t="n">
+        <v>2990</v>
       </c>
     </row>
     <row r="24">
@@ -749,13 +799,16 @@
         <v>45008</v>
       </c>
       <c r="B24" t="n">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C24" t="n">
         <v>472</v>
       </c>
       <c r="D24" t="n">
         <v>95</v>
+      </c>
+      <c r="E24" t="n">
+        <v>3072</v>
       </c>
     </row>
     <row r="25">
@@ -763,13 +816,16 @@
         <v>45009</v>
       </c>
       <c r="B25" t="n">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C25" t="n">
         <v>536</v>
       </c>
       <c r="D25" t="n">
         <v>94</v>
+      </c>
+      <c r="E25" t="n">
+        <v>3120</v>
       </c>
     </row>
     <row r="26">
@@ -791,7 +847,7 @@
         <v>45011</v>
       </c>
       <c r="B27" t="n">
-        <v>-19</v>
+        <v>27</v>
       </c>
       <c r="C27" t="n">
         <v>304</v>
@@ -800,7 +856,7 @@
         <v>36</v>
       </c>
       <c r="E27" t="n">
-        <v>3000</v>
+        <v>3006</v>
       </c>
       <c r="F27" t="n">
         <v>132</v>
@@ -814,13 +870,21 @@
         <v>45012</v>
       </c>
       <c r="B28" t="n">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C28" t="n">
         <v>553</v>
       </c>
       <c r="D28" t="n">
         <v>102</v>
+      </c>
+      <c r="E28" t="n">
+        <v>3232</v>
+      </c>
+      <c r="H28" s="2" t="inlineStr">
+        <is>
+          <t>ФІКЦІЯ, ДОДАНО ШТУЧНО, НЕ Є РЕАЬНИМИ ДАНИМИ</t>
+        </is>
       </c>
     </row>
     <row r="29">
@@ -828,13 +892,16 @@
         <v>45013</v>
       </c>
       <c r="B29" t="n">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C29" t="n">
         <v>412</v>
       </c>
       <c r="D29" t="n">
         <v>67</v>
+      </c>
+      <c r="E29" t="n">
+        <v>3274</v>
       </c>
     </row>
     <row r="30">
@@ -842,13 +909,16 @@
         <v>45014</v>
       </c>
       <c r="B30" t="n">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C30" t="n">
         <v>326</v>
       </c>
       <c r="D30" t="n">
         <v>51</v>
+      </c>
+      <c r="E30" t="n">
+        <v>3314</v>
       </c>
     </row>
     <row r="31">
@@ -856,13 +926,16 @@
         <v>45015</v>
       </c>
       <c r="B31" t="n">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C31" t="n">
         <v>504</v>
       </c>
       <c r="D31" t="n">
         <v>85</v>
+      </c>
+      <c r="E31" t="n">
+        <v>3361</v>
       </c>
     </row>
     <row r="32">
@@ -870,13 +943,16 @@
         <v>45016</v>
       </c>
       <c r="B32" t="n">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="C32" t="n">
         <v>691</v>
       </c>
       <c r="D32" t="n">
         <v>145</v>
+      </c>
+      <c r="E32" t="n">
+        <v>3446</v>
       </c>
     </row>
     <row r="33">
@@ -884,13 +960,16 @@
         <v>45017</v>
       </c>
       <c r="B33" t="n">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C33" t="n">
         <v>426</v>
       </c>
       <c r="D33" t="n">
         <v>81</v>
+      </c>
+      <c r="E33" t="n">
+        <v>3479</v>
       </c>
     </row>
     <row r="34">
@@ -898,13 +977,16 @@
         <v>45018</v>
       </c>
       <c r="B34" t="n">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C34" t="n">
         <v>258</v>
       </c>
       <c r="D34" t="n">
         <v>51</v>
+      </c>
+      <c r="E34" t="n">
+        <v>3502</v>
       </c>
     </row>
     <row r="35">
@@ -912,13 +994,16 @@
         <v>45019</v>
       </c>
       <c r="B35" t="n">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C35" t="n">
         <v>443</v>
       </c>
       <c r="D35" t="n">
         <v>87</v>
+      </c>
+      <c r="E35" t="n">
+        <v>3552</v>
       </c>
     </row>
     <row r="36">
@@ -926,13 +1011,16 @@
         <v>45020</v>
       </c>
       <c r="B36" t="n">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C36" t="n">
         <v>449</v>
       </c>
       <c r="D36" t="n">
         <v>85</v>
+      </c>
+      <c r="E36" t="n">
+        <v>3602</v>
       </c>
     </row>
     <row r="37">
@@ -940,13 +1028,16 @@
         <v>45021</v>
       </c>
       <c r="B37" t="n">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C37" t="n">
         <v>419</v>
       </c>
       <c r="D37" t="n">
         <v>78</v>
+      </c>
+      <c r="E37" t="n">
+        <v>3634</v>
       </c>
     </row>
     <row r="38">
@@ -968,7 +1059,7 @@
         <v>45023</v>
       </c>
       <c r="B39" t="n">
-        <v>15</v>
+        <v>42</v>
       </c>
       <c r="C39" t="n">
         <v>503</v>
@@ -1050,311 +1141,1247 @@
       <c r="A43" s="1" t="n">
         <v>45027</v>
       </c>
+      <c r="B43" t="n">
+        <v>65</v>
+      </c>
+      <c r="C43" t="n">
+        <v>515</v>
+      </c>
+      <c r="D43" t="n">
+        <v>123</v>
+      </c>
+      <c r="E43" t="n">
+        <v>3763</v>
+      </c>
+      <c r="F43" t="n">
+        <v>247</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="n">
         <v>45028</v>
       </c>
+      <c r="B44" t="n">
+        <v>51</v>
+      </c>
+      <c r="C44" t="n">
+        <v>634</v>
+      </c>
+      <c r="D44" t="n">
+        <v>203</v>
+      </c>
+      <c r="E44" t="n">
+        <v>3826</v>
+      </c>
+      <c r="F44" t="n">
+        <v>187</v>
+      </c>
+      <c r="G44" t="n">
+        <v>48</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="n">
         <v>45029</v>
       </c>
+      <c r="B45" t="n">
+        <v>1</v>
+      </c>
+      <c r="C45" t="n">
+        <v>343</v>
+      </c>
+      <c r="D45" t="n">
+        <v>68</v>
+      </c>
+      <c r="E45" t="n">
+        <v>3859</v>
+      </c>
+      <c r="F45" t="n">
+        <v>203</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="n">
         <v>45030</v>
       </c>
+      <c r="B46" t="n">
+        <v>1</v>
+      </c>
+      <c r="C46" t="n">
+        <v>412</v>
+      </c>
+      <c r="D46" t="n">
+        <v>72</v>
+      </c>
+      <c r="E46" t="n">
+        <v>3864</v>
+      </c>
+      <c r="F46" t="n">
+        <v>199</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="n">
         <v>45031</v>
       </c>
+      <c r="B47" t="n">
+        <v>5</v>
+      </c>
+      <c r="C47" t="n">
+        <v>147</v>
+      </c>
+      <c r="D47" t="n">
+        <v>23</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="n">
         <v>45032</v>
       </c>
+      <c r="B48" t="n">
+        <v>32</v>
+      </c>
+      <c r="C48" t="n">
+        <v>234</v>
+      </c>
+      <c r="D48" t="n">
+        <v>51</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="n">
         <v>45033</v>
       </c>
+      <c r="B49" t="n">
+        <v>11</v>
+      </c>
+      <c r="C49" t="n">
+        <v>415</v>
+      </c>
+      <c r="D49" t="n">
+        <v>70</v>
+      </c>
+      <c r="E49" t="n">
+        <v>3978</v>
+      </c>
+      <c r="F49" t="n">
+        <v>130</v>
+      </c>
+      <c r="G49" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="n">
         <v>45034</v>
       </c>
+      <c r="B50" t="n">
+        <v>10</v>
+      </c>
+      <c r="C50" t="n">
+        <v>232</v>
+      </c>
+      <c r="D50" t="n">
+        <v>36</v>
+      </c>
+      <c r="E50" t="n">
+        <v>3987</v>
+      </c>
+      <c r="F50" t="n">
+        <v>134</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="n">
         <v>45035</v>
       </c>
+      <c r="B51" t="n">
+        <v>50</v>
+      </c>
+      <c r="C51" t="n">
+        <v>309</v>
+      </c>
+      <c r="D51" t="n">
+        <v>50</v>
+      </c>
+      <c r="E51" t="n">
+        <v>4033</v>
+      </c>
+      <c r="F51" t="n">
+        <v>138</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="n">
         <v>45036</v>
       </c>
+      <c r="B52" t="n">
+        <v>50</v>
+      </c>
+      <c r="C52" t="n">
+        <v>473</v>
+      </c>
+      <c r="D52" t="n">
+        <v>93</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="n">
         <v>45037</v>
       </c>
+      <c r="B53" t="n">
+        <v>30</v>
+      </c>
+      <c r="C53" t="n">
+        <v>431</v>
+      </c>
+      <c r="D53" t="n">
+        <v>85</v>
+      </c>
+      <c r="E53" t="n">
+        <v>4039</v>
+      </c>
+      <c r="F53" t="n">
+        <v>189</v>
+      </c>
+      <c r="G53" t="n">
+        <v>23</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="n">
         <v>45038</v>
       </c>
+      <c r="B54" t="n">
+        <v>26</v>
+      </c>
+      <c r="C54" t="n">
+        <v>394</v>
+      </c>
+      <c r="D54" t="n">
+        <v>62</v>
+      </c>
+      <c r="E54" t="n">
+        <v>4080</v>
+      </c>
+      <c r="F54" t="n">
+        <v>187</v>
+      </c>
+      <c r="G54" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="n">
         <v>45039</v>
       </c>
+      <c r="B55" t="n">
+        <v>36</v>
+      </c>
+      <c r="C55" t="n">
+        <v>434</v>
+      </c>
+      <c r="D55" t="n">
+        <v>76</v>
+      </c>
+      <c r="E55" t="n">
+        <v>4118</v>
+      </c>
+      <c r="F55" t="n">
+        <v>195</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="n">
         <v>45040</v>
       </c>
+      <c r="B56" t="n">
+        <v>21</v>
+      </c>
+      <c r="C56" t="n">
+        <v>294</v>
+      </c>
+      <c r="D56" t="n">
+        <v>47</v>
+      </c>
+      <c r="E56" t="n">
+        <v>4135</v>
+      </c>
+      <c r="F56" t="n">
+        <v>140</v>
+      </c>
+      <c r="G56" t="n">
+        <v>59</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="n">
         <v>45041</v>
       </c>
+      <c r="B57" t="n">
+        <v>17</v>
+      </c>
+      <c r="C57" t="n">
+        <v>383</v>
+      </c>
+      <c r="D57" t="n">
+        <v>61</v>
+      </c>
+      <c r="E57" t="n">
+        <v>4183</v>
+      </c>
+      <c r="F57" t="n">
+        <v>168</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" s="1" t="n">
         <v>45042</v>
       </c>
+      <c r="B58" t="n">
+        <v>6</v>
+      </c>
+      <c r="C58" t="n">
+        <v>228</v>
+      </c>
+      <c r="D58" t="n">
+        <v>33</v>
+      </c>
+      <c r="E58" t="n">
+        <v>4205</v>
+      </c>
+      <c r="F58" t="n">
+        <v>152</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="n">
         <v>45043</v>
       </c>
+      <c r="B59" t="n">
+        <v>9</v>
+      </c>
+      <c r="C59" t="n">
+        <v>242</v>
+      </c>
+      <c r="D59" t="n">
+        <v>32</v>
+      </c>
+      <c r="E59" t="n">
+        <v>4260</v>
+      </c>
+      <c r="F59" t="n">
+        <v>106</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" s="1" t="n">
         <v>45044</v>
       </c>
+      <c r="B60" t="n">
+        <v>34</v>
+      </c>
+      <c r="C60" t="n">
+        <v>351</v>
+      </c>
+      <c r="D60" t="n">
+        <v>53</v>
+      </c>
+      <c r="E60" t="n">
+        <v>4282</v>
+      </c>
+      <c r="F60" t="n">
+        <v>118</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" s="1" t="n">
         <v>45045</v>
       </c>
+      <c r="B61" t="n">
+        <v>4</v>
+      </c>
+      <c r="C61" t="n">
+        <v>228</v>
+      </c>
+      <c r="D61" t="n">
+        <v>37</v>
+      </c>
+      <c r="E61" t="n">
+        <v>4277</v>
+      </c>
+      <c r="F61" t="n">
+        <v>127</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62" s="1" t="n">
         <v>45046</v>
       </c>
+      <c r="B62" t="n">
+        <v>3</v>
+      </c>
+      <c r="C62" t="n">
+        <v>219</v>
+      </c>
+      <c r="D62" t="n">
+        <v>35</v>
+      </c>
+      <c r="E62" t="n">
+        <v>4282</v>
+      </c>
+      <c r="F62" t="n">
+        <v>125</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="n">
         <v>45047</v>
       </c>
+      <c r="B63" t="n">
+        <v>7</v>
+      </c>
+      <c r="C63" t="n">
+        <v>210</v>
+      </c>
+      <c r="D63" t="n">
+        <v>31</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="n">
         <v>45048</v>
       </c>
+      <c r="B64" t="n">
+        <v>29</v>
+      </c>
+      <c r="C64" t="n">
+        <v>279</v>
+      </c>
+      <c r="D64" t="n">
+        <v>42</v>
+      </c>
+      <c r="E64" t="n">
+        <v>4298</v>
+      </c>
+      <c r="F64" t="n">
+        <v>145</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="n">
         <v>45049</v>
       </c>
+      <c r="B65" t="n">
+        <v>61</v>
+      </c>
+      <c r="C65" t="n">
+        <v>462</v>
+      </c>
+      <c r="D65" t="n">
+        <v>67</v>
+      </c>
+      <c r="E65" t="n">
+        <v>4308</v>
+      </c>
+      <c r="F65" t="n">
+        <v>196</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" s="1" t="n">
         <v>45050</v>
       </c>
+      <c r="B66" t="n">
+        <v>21</v>
+      </c>
+      <c r="C66" t="n">
+        <v>349</v>
+      </c>
+      <c r="D66" t="n">
+        <v>53</v>
+      </c>
     </row>
     <row r="67">
       <c r="A67" s="1" t="n">
         <v>45051</v>
       </c>
+      <c r="B67" t="n">
+        <v>15</v>
+      </c>
+      <c r="C67" t="n">
+        <v>227</v>
+      </c>
+      <c r="D67" t="n">
+        <v>36</v>
+      </c>
     </row>
     <row r="68">
       <c r="A68" s="1" t="n">
         <v>45052</v>
       </c>
+      <c r="B68" t="n">
+        <v>12</v>
+      </c>
+      <c r="C68" t="n">
+        <v>188</v>
+      </c>
+      <c r="D68" t="n">
+        <v>26</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69" s="1" t="n">
         <v>45053</v>
       </c>
+      <c r="B69" t="n">
+        <v>5</v>
+      </c>
+      <c r="C69" t="n">
+        <v>309</v>
+      </c>
+      <c r="D69" t="n">
+        <v>44</v>
+      </c>
+      <c r="E69" t="n">
+        <v>4419</v>
+      </c>
+      <c r="F69" t="n">
+        <v>138</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70" s="1" t="n">
         <v>45054</v>
       </c>
+      <c r="B70" t="n">
+        <v>2</v>
+      </c>
+      <c r="C70" t="n">
+        <v>181</v>
+      </c>
+      <c r="D70" t="n">
+        <v>23</v>
+      </c>
+      <c r="E70" t="n">
+        <v>4405</v>
+      </c>
+      <c r="F70" t="n">
+        <v>140</v>
+      </c>
+      <c r="G70" t="n">
+        <v>14</v>
+      </c>
     </row>
     <row r="71">
       <c r="A71" s="1" t="n">
         <v>45055</v>
       </c>
+      <c r="B71" t="n">
+        <v>37</v>
+      </c>
+      <c r="C71" t="n">
+        <v>372</v>
+      </c>
+      <c r="D71" t="n">
+        <v>54</v>
+      </c>
     </row>
     <row r="72">
       <c r="A72" s="1" t="n">
         <v>45056</v>
       </c>
+      <c r="B72" t="n">
+        <v>7</v>
+      </c>
+      <c r="C72" t="n">
+        <v>267</v>
+      </c>
+      <c r="D72" t="n">
+        <v>36</v>
+      </c>
+      <c r="E72" t="n">
+        <v>4450</v>
+      </c>
+      <c r="F72" t="n">
+        <v>153</v>
+      </c>
     </row>
     <row r="73">
       <c r="A73" s="1" t="n">
         <v>45057</v>
       </c>
+      <c r="B73" t="n">
+        <v>101</v>
+      </c>
+      <c r="C73" t="n">
+        <v>584</v>
+      </c>
+      <c r="D73" t="n">
+        <v>107</v>
+      </c>
+      <c r="E73" t="n">
+        <v>4454</v>
+      </c>
+      <c r="F73" t="n">
+        <v>250</v>
+      </c>
     </row>
     <row r="74">
       <c r="A74" s="1" t="n">
         <v>45058</v>
       </c>
+      <c r="B74" t="n">
+        <v>8</v>
+      </c>
+      <c r="C74" t="n">
+        <v>404</v>
+      </c>
+      <c r="D74" t="n">
+        <v>65</v>
+      </c>
+      <c r="E74" t="n">
+        <v>4492</v>
+      </c>
+      <c r="F74" t="n">
+        <v>220</v>
+      </c>
     </row>
     <row r="75">
       <c r="A75" s="1" t="n">
         <v>45059</v>
       </c>
+      <c r="B75" t="n">
+        <v>60</v>
+      </c>
+      <c r="C75" t="n">
+        <v>386</v>
+      </c>
+      <c r="D75" t="n">
+        <v>67</v>
+      </c>
+      <c r="E75" t="n">
+        <v>4516</v>
+      </c>
+      <c r="F75" t="n">
+        <v>231</v>
+      </c>
+      <c r="G75" t="n">
+        <v>25</v>
+      </c>
     </row>
     <row r="76">
       <c r="A76" s="1" t="n">
         <v>45060</v>
       </c>
+      <c r="B76" t="n">
+        <v>71</v>
+      </c>
+      <c r="C76" t="n">
+        <v>552</v>
+      </c>
+      <c r="D76" t="n">
+        <v>95</v>
+      </c>
+      <c r="E76" t="n">
+        <v>4598</v>
+      </c>
+      <c r="F76" t="n">
+        <v>245</v>
+      </c>
     </row>
     <row r="77">
       <c r="A77" s="1" t="n">
         <v>45061</v>
       </c>
+      <c r="B77" t="n">
+        <v>24</v>
+      </c>
+      <c r="C77" t="n">
+        <v>403</v>
+      </c>
+      <c r="D77" t="n">
+        <v>79</v>
+      </c>
+      <c r="E77" t="n">
+        <v>4661</v>
+      </c>
+      <c r="F77" t="n">
+        <v>193</v>
+      </c>
+      <c r="G77" t="n">
+        <v>13</v>
+      </c>
     </row>
     <row r="78">
       <c r="A78" s="1" t="n">
         <v>45062</v>
       </c>
+      <c r="B78" t="n">
+        <v>28</v>
+      </c>
+      <c r="C78" t="n">
+        <v>351</v>
+      </c>
+      <c r="D78" t="n">
+        <v>59</v>
+      </c>
+      <c r="E78" t="n">
+        <v>4690</v>
+      </c>
+      <c r="F78" t="n">
+        <v>153</v>
+      </c>
+      <c r="G78" t="n">
+        <v>52</v>
+      </c>
     </row>
     <row r="79">
       <c r="A79" s="1" t="n">
         <v>45063</v>
       </c>
+      <c r="B79" t="n">
+        <v>9</v>
+      </c>
+      <c r="C79" t="n">
+        <v>344</v>
+      </c>
+      <c r="D79" t="n">
+        <v>51</v>
+      </c>
     </row>
     <row r="80">
       <c r="A80" s="1" t="n">
         <v>45064</v>
       </c>
+      <c r="B80" t="n">
+        <v>51</v>
+      </c>
+      <c r="C80" t="n">
+        <v>465</v>
+      </c>
+      <c r="D80" t="n">
+        <v>99</v>
+      </c>
+      <c r="E80" t="n">
+        <v>4755</v>
+      </c>
+      <c r="F80" t="n">
+        <v>162</v>
+      </c>
+      <c r="G80" t="n">
+        <v>38</v>
+      </c>
     </row>
     <row r="81">
       <c r="A81" s="1" t="n">
         <v>45065</v>
       </c>
+      <c r="B81" t="n">
+        <v>21</v>
+      </c>
+      <c r="C81" t="n">
+        <v>340</v>
+      </c>
+      <c r="D81" t="n">
+        <v>61</v>
+      </c>
+      <c r="E81" t="n">
+        <v>4788</v>
+      </c>
+      <c r="F81" t="n">
+        <v>188</v>
+      </c>
     </row>
     <row r="82">
       <c r="A82" s="1" t="n">
         <v>45066</v>
       </c>
+      <c r="B82" t="n">
+        <v>36</v>
+      </c>
+      <c r="C82" t="n">
+        <v>367</v>
+      </c>
+      <c r="D82" t="n">
+        <v>65</v>
+      </c>
+      <c r="E82" t="n">
+        <v>4816</v>
+      </c>
+      <c r="F82" t="n">
+        <v>196</v>
+      </c>
     </row>
     <row r="83">
       <c r="A83" s="1" t="n">
         <v>45067</v>
       </c>
+      <c r="B83" t="n">
+        <v>9</v>
+      </c>
+      <c r="C83" t="n">
+        <v>294</v>
+      </c>
+      <c r="D83" t="n">
+        <v>50</v>
+      </c>
+      <c r="E83" t="n">
+        <v>4863</v>
+      </c>
+      <c r="F83" t="n">
+        <v>158</v>
+      </c>
     </row>
     <row r="84">
       <c r="A84" s="1" t="n">
         <v>45068</v>
       </c>
+      <c r="B84" t="n">
+        <v>24</v>
+      </c>
+      <c r="C84" t="n">
+        <v>331</v>
+      </c>
+      <c r="D84" t="n">
+        <v>66</v>
+      </c>
+      <c r="E84" t="n">
+        <v>4873</v>
+      </c>
+      <c r="F84" t="n">
+        <v>172</v>
+      </c>
     </row>
     <row r="85">
       <c r="A85" s="1" t="n">
         <v>45069</v>
       </c>
+      <c r="B85" t="n">
+        <v>6</v>
+      </c>
+      <c r="C85" t="n">
+        <v>206</v>
+      </c>
+      <c r="D85" t="n">
+        <v>30</v>
+      </c>
+      <c r="E85" t="n">
+        <v>4865</v>
+      </c>
+      <c r="F85" t="n">
+        <v>135</v>
+      </c>
+      <c r="G85" t="n">
+        <v>51</v>
+      </c>
     </row>
     <row r="86">
       <c r="A86" s="1" t="n">
         <v>45070</v>
       </c>
+      <c r="B86" t="n">
+        <v>20</v>
+      </c>
+      <c r="C86" t="n">
+        <v>301</v>
+      </c>
+      <c r="D86" t="n">
+        <v>56</v>
+      </c>
+      <c r="E86" t="n">
+        <v>4903</v>
+      </c>
+      <c r="F86" t="n">
+        <v>94</v>
+      </c>
+      <c r="G86" t="n">
+        <v>74</v>
+      </c>
     </row>
     <row r="87">
       <c r="A87" s="1" t="n">
         <v>45071</v>
       </c>
+      <c r="B87" t="n">
+        <v>15</v>
+      </c>
+      <c r="C87" t="n">
+        <v>213</v>
+      </c>
+      <c r="D87" t="n">
+        <v>32</v>
+      </c>
+      <c r="E87" t="n">
+        <v>4906</v>
+      </c>
+      <c r="F87" t="n">
+        <v>98</v>
+      </c>
+      <c r="G87" t="n">
+        <v>82</v>
+      </c>
     </row>
     <row r="88">
       <c r="A88" s="1" t="n">
         <v>45072</v>
       </c>
+      <c r="B88" t="n">
+        <v>25</v>
+      </c>
+      <c r="C88" t="n">
+        <v>326</v>
+      </c>
+      <c r="D88" t="n">
+        <v>56</v>
+      </c>
+      <c r="E88" t="n">
+        <v>4930</v>
+      </c>
+      <c r="F88" t="n">
+        <v>112</v>
+      </c>
+      <c r="G88" t="n">
+        <v>69</v>
+      </c>
     </row>
     <row r="89">
       <c r="A89" s="1" t="n">
         <v>45073</v>
       </c>
+      <c r="B89" t="n">
+        <v>0</v>
+      </c>
+      <c r="C89" t="n">
+        <v>186</v>
+      </c>
+      <c r="D89" t="n">
+        <v>30</v>
+      </c>
+      <c r="E89" t="n">
+        <v>4920</v>
+      </c>
+      <c r="F89" t="n">
+        <v>130</v>
+      </c>
+      <c r="G89" t="n">
+        <v>61</v>
+      </c>
     </row>
     <row r="90">
       <c r="A90" s="1" t="n">
         <v>45074</v>
       </c>
+      <c r="B90" t="n">
+        <v>6</v>
+      </c>
+      <c r="C90" t="n">
+        <v>256</v>
+      </c>
+      <c r="D90" t="n">
+        <v>38</v>
+      </c>
+      <c r="E90" t="n">
+        <v>4919</v>
+      </c>
+      <c r="F90" t="n">
+        <v>80</v>
+      </c>
+      <c r="G90" t="n">
+        <v>118</v>
+      </c>
     </row>
     <row r="91">
       <c r="A91" s="1" t="n">
         <v>45075</v>
       </c>
+      <c r="B91" t="n">
+        <v>69</v>
+      </c>
+      <c r="C91" t="n">
+        <v>387</v>
+      </c>
+      <c r="D91" t="n">
+        <v>74</v>
+      </c>
     </row>
     <row r="92">
       <c r="A92" s="1" t="n">
         <v>45076</v>
       </c>
+      <c r="B92" t="n">
+        <v>7</v>
+      </c>
+      <c r="C92" t="n">
+        <v>416</v>
+      </c>
+      <c r="D92" t="n">
+        <v>71</v>
+      </c>
+      <c r="E92" t="n">
+        <v>4997</v>
+      </c>
+      <c r="F92" t="n">
+        <v>196</v>
+      </c>
     </row>
     <row r="93">
       <c r="A93" s="1" t="n">
         <v>45077</v>
       </c>
+      <c r="B93" t="n">
+        <v>26</v>
+      </c>
+      <c r="C93" t="n">
+        <v>341</v>
+      </c>
+      <c r="D93" t="n">
+        <v>53</v>
+      </c>
+      <c r="E93" t="n">
+        <v>5014</v>
+      </c>
+      <c r="F93" t="n">
+        <v>141</v>
+      </c>
+      <c r="G93" t="n">
+        <v>64</v>
+      </c>
     </row>
     <row r="94">
       <c r="A94" s="1" t="n">
         <v>45078</v>
       </c>
+      <c r="B94" t="n">
+        <v>36</v>
+      </c>
+      <c r="C94" t="n">
+        <v>470</v>
+      </c>
+      <c r="D94" t="n">
+        <v>92</v>
+      </c>
+      <c r="E94" t="n">
+        <v>5056</v>
+      </c>
+      <c r="F94" t="n">
+        <v>143</v>
+      </c>
+      <c r="G94" t="n">
+        <v>56</v>
+      </c>
     </row>
     <row r="95">
       <c r="A95" s="1" t="n">
         <v>45079</v>
       </c>
+      <c r="B95" t="n">
+        <v>20</v>
+      </c>
+      <c r="C95" t="n">
+        <v>318</v>
+      </c>
+      <c r="D95" t="n">
+        <v>68</v>
+      </c>
+      <c r="E95" t="n">
+        <v>5087</v>
+      </c>
+      <c r="F95" t="n">
+        <v>174</v>
+      </c>
+      <c r="G95" t="n">
+        <v>14</v>
+      </c>
     </row>
     <row r="96">
       <c r="A96" s="1" t="n">
         <v>45080</v>
       </c>
+      <c r="B96" t="n">
+        <v>11</v>
+      </c>
+      <c r="C96" t="n">
+        <v>332</v>
+      </c>
+      <c r="D96" t="n">
+        <v>53</v>
+      </c>
+      <c r="E96" t="n">
+        <v>5113</v>
+      </c>
+      <c r="F96" t="n">
+        <v>139</v>
+      </c>
+      <c r="G96" t="n">
+        <v>34</v>
+      </c>
     </row>
     <row r="97">
       <c r="A97" s="1" t="n">
         <v>45081</v>
       </c>
+      <c r="B97" t="n">
+        <v>8</v>
+      </c>
+      <c r="C97" t="n">
+        <v>219</v>
+      </c>
+      <c r="D97" t="n">
+        <v>34</v>
+      </c>
+      <c r="E97" t="n">
+        <v>5117</v>
+      </c>
+      <c r="F97" t="n">
+        <v>117</v>
+      </c>
+      <c r="G97" t="n">
+        <v>60</v>
+      </c>
     </row>
     <row r="98">
       <c r="A98" s="1" t="n">
         <v>45082</v>
       </c>
+      <c r="B98" t="n">
+        <v>0</v>
+      </c>
+      <c r="C98" t="n">
+        <v>280</v>
+      </c>
+      <c r="D98" t="n">
+        <v>46</v>
+      </c>
+      <c r="E98" t="n">
+        <v>5173</v>
+      </c>
+      <c r="F98" t="n">
+        <v>92</v>
+      </c>
+      <c r="G98" t="n">
+        <v>29</v>
+      </c>
     </row>
     <row r="99">
       <c r="A99" s="1" t="n">
         <v>45083</v>
       </c>
+      <c r="B99" t="n">
+        <v>9</v>
+      </c>
+      <c r="C99" t="n">
+        <v>186</v>
+      </c>
+      <c r="D99" t="n">
+        <v>37</v>
+      </c>
+      <c r="E99" t="n">
+        <v>5172</v>
+      </c>
+      <c r="F99" t="n">
+        <v>115</v>
+      </c>
+      <c r="G99" t="n">
+        <v>16</v>
+      </c>
     </row>
     <row r="100">
       <c r="A100" s="1" t="n">
         <v>45084</v>
       </c>
+      <c r="B100" t="n">
+        <v>23</v>
+      </c>
+      <c r="C100" t="n">
+        <v>240</v>
+      </c>
+      <c r="D100" t="n">
+        <v>44</v>
+      </c>
+      <c r="E100" t="n">
+        <v>5160</v>
+      </c>
+      <c r="F100" t="n">
+        <v>96</v>
+      </c>
+      <c r="G100" t="n">
+        <v>70</v>
+      </c>
     </row>
     <row r="101">
       <c r="A101" s="1" t="n">
         <v>45085</v>
       </c>
+      <c r="B101" t="n">
+        <v>9</v>
+      </c>
+      <c r="C101" t="n">
+        <v>196</v>
+      </c>
+      <c r="D101" t="n">
+        <v>30</v>
+      </c>
+      <c r="E101" t="n">
+        <v>5159</v>
+      </c>
+      <c r="F101" t="n">
+        <v>75</v>
+      </c>
+      <c r="G101" t="n">
+        <v>101</v>
+      </c>
     </row>
     <row r="102">
       <c r="A102" s="1" t="n">
         <v>45086</v>
       </c>
+      <c r="B102" t="n">
+        <v>4</v>
+      </c>
+      <c r="C102" t="n">
+        <v>141</v>
+      </c>
+      <c r="D102" t="n">
+        <v>21</v>
+      </c>
+      <c r="E102" t="n">
+        <v>5125</v>
+      </c>
+      <c r="F102" t="n">
+        <v>89</v>
+      </c>
+      <c r="G102" t="n">
+        <v>125</v>
+      </c>
     </row>
     <row r="103">
       <c r="A103" s="1" t="n">
         <v>45087</v>
       </c>
+      <c r="B103" t="n">
+        <v>0</v>
+      </c>
+      <c r="C103" t="n">
+        <v>218</v>
+      </c>
+      <c r="D103" t="n">
+        <v>35</v>
+      </c>
     </row>
     <row r="104">
       <c r="A104" s="1" t="n">
         <v>45088</v>
       </c>
+      <c r="B104" t="n">
+        <v>0</v>
+      </c>
+      <c r="C104" t="n">
+        <v>270</v>
+      </c>
+      <c r="D104" t="n">
+        <v>34</v>
+      </c>
     </row>
     <row r="105">
       <c r="A105" s="1" t="n">
@@ -6362,6 +7389,10 @@
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="H11:H26"/>
+    <mergeCell ref="H28:H38"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>